<commit_message>
Checking code on 27th mar 19
</commit_message>
<xml_diff>
--- a/DataSheets/Login.xlsx
+++ b/DataSheets/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vishal\SMART_AUTO\DataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vishal\SMART_Automation\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C87F4EE-2A5A-4B53-9A3A-53FF84661D02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C910488F-5B39-41D0-9A66-850DE50ADF39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid" sheetId="2" r:id="rId1"/>
@@ -111,7 +111,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>